<commit_message>
feat: add ELO and MVP simulation Excel tool
Updated `ELO_Simulation.xlsx` to include MVP scoring simulations.
Updated `scripts/generate_elo_sim.py` to support new MVP sheets.

The updated Excel file includes:
- ELO Match Simulator (Single Match, Scenarios, Sequence).
- MVP Scoring Simulator (Standard and Rolling scores).
- MVP Scenarios (Efficiency King, Workhorse, Comeback).
- Detailed documentation for both ELO and MVP logic.
</commit_message>
<xml_diff>
--- a/ELO_Simulation.xlsx
+++ b/ELO_Simulation.xlsx
@@ -10,7 +10,9 @@
     <sheet name="Single Match Simulator" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Scenarios" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sequence Simulator" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Documentation" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MVP Simulator" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MVP Scenarios" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Documentation" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1675,7 +1677,612 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>MVP Scoring Simulator</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t>Player Name</t>
+        </is>
+      </c>
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>ELO Gain</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>Games Played</t>
+        </is>
+      </c>
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>Win Rate</t>
+        </is>
+      </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>Total ELO</t>
+        </is>
+      </c>
+      <c r="G3" s="9" t="inlineStr">
+        <is>
+          <t>Eligibility</t>
+        </is>
+      </c>
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>Standard MVP Score</t>
+        </is>
+      </c>
+      <c r="I3" s="9" t="inlineStr">
+        <is>
+          <t>Rolling MVP Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Player 1</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5">
+        <f>IF(D4=0, 0, C4/D4)</f>
+        <v/>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G4" s="7">
+        <f>IF(D4&gt;=6, "Month OK", IF(D4&gt;=3, "Evening OK", "Too few games"))</f>
+        <v/>
+      </c>
+      <c r="H4" s="7">
+        <f>B4 * (0.9 + 0.2 * E4) + 0.3 * D4</f>
+        <v/>
+      </c>
+      <c r="I4" s="7">
+        <f>C4 * 3 + E4 * 5 + D4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Player 2</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <f>IF(D5=0, 0, C5/D5)</f>
+        <v/>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G5" s="7">
+        <f>IF(D5&gt;=6, "Month OK", IF(D5&gt;=3, "Evening OK", "Too few games"))</f>
+        <v/>
+      </c>
+      <c r="H5" s="7">
+        <f>B5 * (0.9 + 0.2 * E5) + 0.3 * D5</f>
+        <v/>
+      </c>
+      <c r="I5" s="7">
+        <f>C5 * 3 + E5 * 5 + D5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Player 3</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5">
+        <f>IF(D6=0, 0, C6/D6)</f>
+        <v/>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G6" s="7">
+        <f>IF(D6&gt;=6, "Month OK", IF(D6&gt;=3, "Evening OK", "Too few games"))</f>
+        <v/>
+      </c>
+      <c r="H6" s="7">
+        <f>B6 * (0.9 + 0.2 * E6) + 0.3 * D6</f>
+        <v/>
+      </c>
+      <c r="I6" s="7">
+        <f>C6 * 3 + E6 * 5 + D6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Player 4</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5">
+        <f>IF(D7=0, 0, C7/D7)</f>
+        <v/>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G7" s="7">
+        <f>IF(D7&gt;=6, "Month OK", IF(D7&gt;=3, "Evening OK", "Too few games"))</f>
+        <v/>
+      </c>
+      <c r="H7" s="7">
+        <f>B7 * (0.9 + 0.2 * E7) + 0.3 * D7</f>
+        <v/>
+      </c>
+      <c r="I7" s="7">
+        <f>C7 * 3 + E7 * 5 + D7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>Player 5</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5">
+        <f>IF(D8=0, 0, C8/D8)</f>
+        <v/>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G8" s="7">
+        <f>IF(D8&gt;=6, "Month OK", IF(D8&gt;=3, "Evening OK", "Too few games"))</f>
+        <v/>
+      </c>
+      <c r="H8" s="7">
+        <f>B8 * (0.9 + 0.2 * E8) + 0.3 * D8</f>
+        <v/>
+      </c>
+      <c r="I8" s="7">
+        <f>C8 * 3 + E8 * 5 + D8</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Scenario 1: The Efficiency King</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>High win rate, few games (Evening MVP focus).</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>ELO Gain</t>
+        </is>
+      </c>
+      <c r="C2" s="9" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D2" s="9" t="inlineStr">
+        <is>
+          <t>Games</t>
+        </is>
+      </c>
+      <c r="E2" s="9" t="inlineStr">
+        <is>
+          <t>Win Rate</t>
+        </is>
+      </c>
+      <c r="F2" s="9" t="inlineStr">
+        <is>
+          <t>Std MVP Score</t>
+        </is>
+      </c>
+      <c r="G2" s="9" t="inlineStr">
+        <is>
+          <t>Roll MVP Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Efficiency King</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>44.9</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>The Grinder</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>32.8</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>21.33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr"/>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="5" t="inlineStr"/>
+      <c r="E5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>Scenario 2: The Workhorse</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>High game count compensates for lower efficiency (Month MVP focus).</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B7" s="9" t="inlineStr">
+        <is>
+          <t>ELO Gain</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>Games</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="inlineStr">
+        <is>
+          <t>Win Rate</t>
+        </is>
+      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>Std MVP Score</t>
+        </is>
+      </c>
+      <c r="G7" s="9" t="inlineStr">
+        <is>
+          <t>Roll MVP Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Workhorse</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>55</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>Elite Sprinter</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>25.17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr"/>
+      <c r="B10" s="5" t="inlineStr"/>
+      <c r="C10" s="5" t="inlineStr"/>
+      <c r="D10" s="5" t="inlineStr"/>
+      <c r="E10" s="5" t="inlineStr"/>
+      <c r="F10" s="5" t="inlineStr"/>
+      <c r="G10" s="5" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>Scenario 3: The Comeback</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>Massive ELO gains from underdog wins.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>ELO Gain</t>
+        </is>
+      </c>
+      <c r="C12" s="9" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D12" s="9" t="inlineStr">
+        <is>
+          <t>Games</t>
+        </is>
+      </c>
+      <c r="E12" s="9" t="inlineStr">
+        <is>
+          <t>Win Rate</t>
+        </is>
+      </c>
+      <c r="F12" s="9" t="inlineStr">
+        <is>
+          <t>Std MVP Score</t>
+        </is>
+      </c>
+      <c r="G12" s="9" t="inlineStr">
+        <is>
+          <t>Roll MVP Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Underdog Hero</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>85.2</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>Consistent Pro</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1800,43 +2407,125 @@
       <c r="B10" s="5" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Excel Formulas used:</t>
-        </is>
-      </c>
-      <c r="B11" s="5" t="inlineStr"/>
+      <c r="A11" s="11" t="inlineStr">
+        <is>
+          <t>MVP Scoring</t>
+        </is>
+      </c>
+      <c r="B11" s="11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>Expected Score</t>
-        </is>
-      </c>
-      <c r="B12" s="5">
-        <f>1 / (1 + 10^((Opponent_Avg - Own_Avg) / 300))</f>
-        <v/>
+          <t>Standard MVP Score</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>Used for Evening and Month MVP awards.</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Player Weight</t>
-        </is>
-      </c>
-      <c r="B13" s="5">
-        <f>MIN(1.25, MAX(0.75, 1 + (Team_Avg - Player_Elo) / 800))</f>
-        <v/>
+          <t>Rolling MVP Score</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Used for the 'MVP Days' counter in player profiles.</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>Delta</t>
-        </is>
-      </c>
-      <c r="B14" s="5">
+          <t>Evening MVP Eligibility</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Must play at least 3 matches in the session.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Month MVP Eligibility</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Must play at least 6 matches in the rolling 30-day window.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr"/>
+      <c r="B16" s="5" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="inlineStr">
+        <is>
+          <t>Excel Formulas used:</t>
+        </is>
+      </c>
+      <c r="B17" s="11" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Expected Score</t>
+        </is>
+      </c>
+      <c r="B18" s="5">
+        <f>1 / (1 + 10^((Opponent_Avg - Own_Avg) / 300))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>Player Weight</t>
+        </is>
+      </c>
+      <c r="B19" s="5">
+        <f>MIN(1.25, MAX(0.75, 1 + (Team_Avg - Player_Elo) / 800))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>Delta (ELO)</t>
+        </is>
+      </c>
+      <c r="B20" s="5">
         <f>ROUND(K * MarginMult * MatchWeight * EffWeight * (Result - Expected), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Standard MVP Score</t>
+        </is>
+      </c>
+      <c r="B21" s="5">
+        <f>eloGain * (0.9 + 0.2 * winRate) + 0.3 * gamesPlayed</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>Rolling MVP Score</t>
+        </is>
+      </c>
+      <c r="B22" s="5">
+        <f>wins * 3 + winRate * 5 + gamesPlayed</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Harmonize MVP calculations and improve scoring formula
- Created centralized src/utils/mvp.ts for MVP scoring and winner selection.
- Updated Dashboard and Profile MVP counters to use the same logic.
- Implemented new additive formula: Score = eloGain + (winRate * 15) + (games * 0.5).
- Renamed "MVP-månader" to "MVP-dagar (Månad)" in profile.
- Updated documentation in docs/MVP_CALCULATIONS.md.
- Updated simulation script scripts/generate_elo_sim.py.
- Added unit tests in src/utils/mvp.test.ts.
</commit_message>
<xml_diff>
--- a/ELO_Simulation.xlsx
+++ b/ELO_Simulation.xlsx
@@ -1777,11 +1777,11 @@
         <v/>
       </c>
       <c r="H4" s="7">
-        <f>B4 * (0.9 + 0.2 * E4) + 0.3 * D4</f>
+        <f>B4 + (E4 * 15) + (D4 * 0.5)</f>
         <v/>
       </c>
       <c r="I4" s="7">
-        <f>C4 * 3 + E4 * 5 + D4</f>
+        <f>H4</f>
         <v/>
       </c>
     </row>
@@ -1812,11 +1812,11 @@
         <v/>
       </c>
       <c r="H5" s="7">
-        <f>B5 * (0.9 + 0.2 * E5) + 0.3 * D5</f>
+        <f>B5 + (E5 * 15) + (D5 * 0.5)</f>
         <v/>
       </c>
       <c r="I5" s="7">
-        <f>C5 * 3 + E5 * 5 + D5</f>
+        <f>H5</f>
         <v/>
       </c>
     </row>
@@ -1847,11 +1847,11 @@
         <v/>
       </c>
       <c r="H6" s="7">
-        <f>B6 * (0.9 + 0.2 * E6) + 0.3 * D6</f>
+        <f>B6 + (E6 * 15) + (D6 * 0.5)</f>
         <v/>
       </c>
       <c r="I6" s="7">
-        <f>C6 * 3 + E6 * 5 + D6</f>
+        <f>H6</f>
         <v/>
       </c>
     </row>
@@ -1882,11 +1882,11 @@
         <v/>
       </c>
       <c r="H7" s="7">
-        <f>B7 * (0.9 + 0.2 * E7) + 0.3 * D7</f>
+        <f>B7 + (E7 * 15) + (D7 * 0.5)</f>
         <v/>
       </c>
       <c r="I7" s="7">
-        <f>C7 * 3 + E7 * 5 + D7</f>
+        <f>H7</f>
         <v/>
       </c>
     </row>
@@ -1917,11 +1917,11 @@
         <v/>
       </c>
       <c r="H8" s="7">
-        <f>B8 * (0.9 + 0.2 * E8) + 0.3 * D8</f>
+        <f>B8 + (E8 * 15) + (D8 * 0.5)</f>
         <v/>
       </c>
       <c r="I8" s="7">
-        <f>C8 * 3 + E8 * 5 + D8</f>
+        <f>H8</f>
         <v/>
       </c>
     </row>
@@ -2024,10 +2024,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>44.9</v>
+        <v>56.5</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>17</v>
+        <v>56.5</v>
       </c>
     </row>
     <row r="4">
@@ -2049,10 +2049,10 @@
         <v>0.67</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>32.8</v>
+        <v>43.05</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>21.33</v>
+        <v>43.05</v>
       </c>
     </row>
     <row r="5">
@@ -2132,10 +2132,10 @@
         <v>0.7</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>55</v>
+        <v>65.5</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>34.5</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="9">
@@ -2157,10 +2157,10 @@
         <v>0.83</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>65.8</v>
+        <v>75.45</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>25.17</v>
+        <v>75.45</v>
       </c>
     </row>
     <row r="10">
@@ -2240,10 +2240,10 @@
         <v>0.75</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>85.2</v>
+        <v>93.25</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>16.75</v>
+        <v>93.25</v>
       </c>
     </row>
     <row r="14">
@@ -2265,10 +2265,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>45.5</v>
+        <v>57.5</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>25</v>
+        <v>57.5</v>
       </c>
     </row>
   </sheetData>
@@ -2429,12 +2429,12 @@
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Rolling MVP Score</t>
+          <t>MVP Days Score</t>
         </is>
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>Used for the 'MVP Days' counter in player profiles.</t>
+          <t>Now harmonized with the Standard MVP Score.</t>
         </is>
       </c>
     </row>
@@ -2514,18 +2514,18 @@
         </is>
       </c>
       <c r="B21" s="5">
-        <f>eloGain * (0.9 + 0.2 * winRate) + 0.3 * gamesPlayed</f>
+        <f>eloGain + (winRate * 15) + (gamesPlayed * 0.5)</f>
         <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Rolling MVP Score</t>
+          <t>MVP Days Score</t>
         </is>
       </c>
       <c r="B22" s="5">
-        <f>wins * 3 + winRate * 5 + gamesPlayed</f>
+        <f>eloGain + (winRate * 15) + (gamesPlayed * 0.5)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: update ELO documentation and simulation tool for singles matches
- Update ELO_CALCULATIONS.md to include Singles Match Weight (0.5x).
- Update scripts/generate_elo_sim.py to support Singles match simulation.
- Regenerate ELO_Simulation.xlsx with the new logic.
- Ensure all ELO documentation reflects current engine behavior.

Co-authored-by: SoMedNinja <198326581+SoMedNinja@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ELO_Simulation.xlsx
+++ b/ELO_Simulation.xlsx
@@ -570,6 +570,23 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Is Singles?</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1v1 matches count 0.5x weight</t>
+        </is>
+      </c>
+    </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
@@ -711,7 +728,7 @@
         <v/>
       </c>
       <c r="L14" s="6">
-        <f>IF(B6="Yes", 1, IF(B4="Sets", IF(MAX(B8,B9)&gt;=6, 1, 0.5), IF(B5&gt;21, 1, 0.5)))</f>
+        <f>IF(B7="Yes", 0.5, 1) * IF(B6="Yes", 1, IF(B4="Sets", IF(MAX(B8,B9)&gt;=6, 1, 0.5), IF(B5&gt;21, 1, 0.5)))</f>
         <v/>
       </c>
       <c r="N14" s="5">
@@ -905,11 +922,14 @@
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Sets,Points"</formula1>
     </dataValidation>
     <dataValidation sqref="B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2282,7 +2302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2369,162 +2389,174 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Player Weight</t>
+          <t>Singles Match Weight</t>
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>Adjusts gain based on partner difference. Lower rated players get a boost (0.75x to 1.25x).</t>
+          <t>1v1 matches count for 0.5x weight.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Effective Weight</t>
+          <t>Player Weight</t>
         </is>
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>Uses Player Weight for wins and 1/Weight for losses.</t>
+          <t>Adjusts gain based on partner difference. Lower rated players get a boost (0.75x to 1.25x).</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
+          <t>Effective Weight</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>Uses Player Weight for wins and 1/Weight for losses.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
           <t>Guest Players</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>The app ignores players marked as Guests. In this simulator, simply leave their ELO blank to exclude them from team averages.</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr"/>
-      <c r="B10" s="5" t="inlineStr"/>
-    </row>
     <row r="11">
-      <c r="A11" s="11" t="inlineStr">
+      <c r="A11" s="4" t="inlineStr"/>
+      <c r="B11" s="5" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="inlineStr">
         <is>
           <t>MVP Scoring</t>
         </is>
       </c>
-      <c r="B11" s="11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Standard MVP Score</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="inlineStr">
-        <is>
-          <t>Used for Evening and Month MVP awards.</t>
-        </is>
-      </c>
+      <c r="B12" s="11" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>MVP Days Score</t>
+          <t>Standard MVP Score</t>
         </is>
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>Now harmonized with the Standard MVP Score.</t>
+          <t>Used for Evening and Month MVP awards.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>Evening MVP Eligibility</t>
+          <t>MVP Days Score</t>
         </is>
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>Must play at least 3 matches in the session.</t>
+          <t>Now harmonized with the Standard MVP Score.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
+          <t>Evening MVP Eligibility</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Must play at least 3 matches in the session.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
           <t>Month MVP Eligibility</t>
         </is>
       </c>
-      <c r="B15" s="5" t="inlineStr">
+      <c r="B16" s="5" t="inlineStr">
         <is>
           <t>Must play at least 6 matches in the rolling 30-day window.</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr"/>
-      <c r="B16" s="5" t="inlineStr"/>
-    </row>
     <row r="17">
-      <c r="A17" s="11" t="inlineStr">
+      <c r="A17" s="4" t="inlineStr"/>
+      <c r="B17" s="5" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="inlineStr">
         <is>
           <t>Excel Formulas used:</t>
         </is>
       </c>
-      <c r="B17" s="11" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>Expected Score</t>
-        </is>
-      </c>
-      <c r="B18" s="5">
-        <f>1 / (1 + 10^((Opponent_Avg - Own_Avg) / 300))</f>
-        <v/>
-      </c>
+      <c r="B18" s="11" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>Player Weight</t>
+          <t>Expected Score</t>
         </is>
       </c>
       <c r="B19" s="5">
-        <f>MIN(1.25, MAX(0.75, 1 + (Team_Avg - Player_Elo) / 800))</f>
+        <f>1 / (1 + 10^((Opponent_Avg - Own_Avg) / 300))</f>
         <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Delta (ELO)</t>
+          <t>Player Weight</t>
         </is>
       </c>
       <c r="B20" s="5">
-        <f>ROUND(K * MarginMult * MatchWeight * EffWeight * (Result - Expected), 0)</f>
+        <f>MIN(1.25, MAX(0.75, 1 + (Team_Avg - Player_Elo) / 800))</f>
         <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Standard MVP Score</t>
+          <t>Delta (ELO)</t>
         </is>
       </c>
       <c r="B21" s="5">
-        <f>eloGain + (winRate * 15) + (gamesPlayed * 0.5)</f>
+        <f>ROUND(K * MarginMult * MatchWeight * SinglesWeight * EffWeight * (Result - Expected), 0)</f>
         <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
+          <t>Standard MVP Score</t>
+        </is>
+      </c>
+      <c r="B22" s="5">
+        <f>eloGain + (winRate * 15) + (gamesPlayed * 0.5)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
           <t>MVP Days Score</t>
         </is>
       </c>
-      <c r="B22" s="5">
+      <c r="B23" s="5">
         <f>eloGain + (winRate * 15) + (gamesPlayed * 0.5)</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
feat: update ELO margin multiplier logic and documentation
- Modify getMarginMultiplier to treat 1 and 2 set differences as equivalent (1.1x multiplier).
- Update ELO_CALCULATIONS.md with new rules and recalculated examples.
- Update scripts/generate_elo_sim.py and regenerate ELO_Simulation.xlsx.
- Update ELO tests to match new algorithm and handle rounding variations.

Co-authored-by: SoMedNinja <198326581+SoMedNinja@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ELO_Simulation.xlsx
+++ b/ELO_Simulation.xlsx
@@ -724,7 +724,7 @@
         <v/>
       </c>
       <c r="K14" s="6">
-        <f>1 + MIN(0.2, MIN(2, ABS(B8 - B9)) * 0.1)</f>
+        <f>1 + IF(ABS(B8-B9)&gt;2, 0.2, IF(ABS(B8-B9)&gt;0, 0.1, 0))</f>
         <v/>
       </c>
       <c r="L14" s="6">
@@ -2302,7 +2302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>Bonus for decisive wins. 2-0 sets = 1.2x multiplier. 2-1 sets = 1.1x.</t>
+          <t>Bonus for decisive wins. 1-2 sets = 1.1x multiplier. 3+ sets = 1.2x.</t>
         </is>
       </c>
     </row>
@@ -2531,32 +2531,43 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Delta (ELO)</t>
+          <t>Margin Multiplier</t>
         </is>
       </c>
       <c r="B21" s="5">
-        <f>ROUND(K * MarginMult * MatchWeight * SinglesWeight * EffWeight * (Result - Expected), 0)</f>
+        <f>1 + IF(ABS(Set_Diff)&gt;2, 0.2, IF(ABS(Set_Diff)&gt;0, 0.1, 0))</f>
         <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Standard MVP Score</t>
+          <t>Delta (ELO)</t>
         </is>
       </c>
       <c r="B22" s="5">
-        <f>eloGain + (winRate * 15) + (gamesPlayed * 0.5)</f>
+        <f>ROUND(K * MarginMult * MatchWeight * SinglesWeight * EffWeight * (Result - Expected), 0)</f>
         <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
+          <t>Standard MVP Score</t>
+        </is>
+      </c>
+      <c r="B23" s="5">
+        <f>eloGain + (winRate * 15) + (gamesPlayed * 0.5)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
           <t>MVP Days Score</t>
         </is>
       </c>
-      <c r="B23" s="5">
+      <c r="B24" s="5">
         <f>eloGain + (winRate * 15) + (gamesPlayed * 0.5)</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
feat: add Scenario 4 (Carry Loss) to ELO simulations and documentation
- Created `ELO_simulations.md` with Scenarios 1-4.
- Added Example 4 (Mixed Team Ratings Loss) to `docs/ELO_CALCULATIONS.md`.
- Updated `scripts/generate_elo_sim.py` with Scenario 4.
- Regenerated `ELO_Simulation.xlsx` with the new scenario.
- Verified changes and confirmed ELO logic tests pass.

Co-authored-by: SoMedNinja <198326581+SoMedNinja@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ELO_Simulation.xlsx
+++ b/ELO_Simulation.xlsx
@@ -943,7 +943,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1447,6 +1447,172 @@
       </c>
       <c r="G20" s="5" t="n">
         <v>993</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr"/>
+      <c r="B21" s="5" t="inlineStr"/>
+      <c r="C21" s="5" t="inlineStr"/>
+      <c r="D21" s="5" t="inlineStr"/>
+      <c r="E21" s="5" t="inlineStr"/>
+      <c r="F21" s="5" t="inlineStr"/>
+      <c r="G21" s="5" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>Scenario 4: Carry (Loss)</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>T1: P1A(1400) &amp; P1B(600) vs T2: Avg 1000. 0-2 Loss for T1.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B23" s="9" t="inlineStr">
+        <is>
+          <t>Start ELO</t>
+        </is>
+      </c>
+      <c r="C23" s="9" t="inlineStr">
+        <is>
+          <t>Games</t>
+        </is>
+      </c>
+      <c r="D23" s="9" t="inlineStr">
+        <is>
+          <t>Opp. Avg</t>
+        </is>
+      </c>
+      <c r="E23" s="9" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="F23" s="9" t="inlineStr">
+        <is>
+          <t>Delta</t>
+        </is>
+      </c>
+      <c r="G23" s="9" t="inlineStr">
+        <is>
+          <t>End ELO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>P1A (1400)</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>1400</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E24" s="5" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>-11</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>P1B (600)</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>600</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E25" s="5" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>-4</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>P2A (1000)</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C26" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D26" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="5" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G26" s="5" t="n">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>P2B (1000)</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G27" s="5" t="n">
+        <v>1007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>